<commit_message>
all momentum sizing functions v and v
</commit_message>
<xml_diff>
--- a/test/ref_Sub_Output.xlsx
+++ b/test/ref_Sub_Output.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\DSE-Mars-Reveal\project\subsystems_design\AOCS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\lmaio\Nextcloud\TU Delft\2019-2020\DSE-Mars-Reveal\project\subsystems_design\AOCS\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1245" yWindow="1830" windowWidth="20370" windowHeight="13020" firstSheet="10" activeTab="10"/>
+    <workbookView xWindow="1245" yWindow="1830" windowWidth="14115" windowHeight="9750" tabRatio="655" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="EPS" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,8 @@
     <sheet name="Payload" sheetId="8" r:id="rId8"/>
     <sheet name="Planetary" sheetId="9" r:id="rId9"/>
     <sheet name="Astro" sheetId="10" r:id="rId10"/>
-    <sheet name="AOCS" sheetId="11" r:id="rId11"/>
+    <sheet name="FireSat" sheetId="12" r:id="rId11"/>
+    <sheet name="AOCS" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="206">
   <si>
     <t>name</t>
   </si>
@@ -624,6 +625,39 @@
   </si>
   <si>
     <t>degrees</t>
+  </si>
+  <si>
+    <t>mass</t>
+  </si>
+  <si>
+    <t>dipole</t>
+  </si>
+  <si>
+    <t>cg</t>
+  </si>
+  <si>
+    <t>c_pres aero</t>
+  </si>
+  <si>
+    <t>c_pres solar</t>
+  </si>
+  <si>
+    <t>solar incidence</t>
+  </si>
+  <si>
+    <t>pt excursion</t>
+  </si>
+  <si>
+    <t>Cd</t>
+  </si>
+  <si>
+    <t>xdim</t>
+  </si>
+  <si>
+    <t>ydim</t>
+  </si>
+  <si>
+    <t>zdim</t>
   </si>
 </sst>
 </file>
@@ -642,11 +676,13 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1344,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,7 +1407,7 @@
         <v>32</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="C2" t="s">
         <v>33</v>
@@ -1490,9 +1526,116 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>197</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>203</v>
+      </c>
+      <c r="B10">
+        <v>1.294</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>204</v>
+      </c>
+      <c r="B11">
+        <v>1.8299799999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B12">
+        <v>1.294</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>

</xml_diff>